<commit_message>
feat: Add initial dashboard HTML, raw data file, and .gitignore configuration.
</commit_message>
<xml_diff>
--- a/data/raw/ponte_2023.xlsx
+++ b/data/raw/ponte_2023.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Documents\Portfolio_perso\Barbara\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Documents\Portfolio_perso\Barbara\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78846181-EBC5-47B9-8B71-B6AAB2E5B67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B07C7BA-0518-46D7-B19D-2AAE870FEEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{DEEF528F-C601-45F0-AE07-540032D5D02C}"/>
+    <workbookView xWindow="0" yWindow="-206" windowWidth="21943" windowHeight="13200" xr2:uid="{DEEF528F-C601-45F0-AE07-540032D5D02C}"/>
   </bookViews>
   <sheets>
     <sheet name="ponte_2023" sheetId="1" r:id="rId1"/>

</xml_diff>